<commit_message>
add req car by id msg
</commit_message>
<xml_diff>
--- a/docs/excel/proto_index.xlsx
+++ b/docs/excel/proto_index.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="248">
   <si>
     <t>Id</t>
   </si>
@@ -106,7 +106,13 @@
     <t>msg.C2GW_ReqCarInfo</t>
   </si>
   <si>
+    <t>msg.C2GW_ReqCarInfoById</t>
+  </si>
+  <si>
     <t>msg.GW2C_ResCarInfo</t>
+  </si>
+  <si>
+    <t>msg.GW2C_ResCarInfoById</t>
   </si>
   <si>
     <t>msg.C2GW_ReqMyParkingInfo</t>
@@ -1133,7 +1139,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B226"/>
+  <dimension ref="A1:B228"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -2949,6 +2955,22 @@
       </c>
       <c r="B226" s="1" t="s">
         <v>228</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="1">
+        <v>223</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="1">
+        <v>224</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -2987,59 +3009,59 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>